<commit_message>
tree app Daten eingefügt
</commit_message>
<xml_diff>
--- a/SO_nais_einheiten_unique.xlsx
+++ b/SO_nais_einheiten_unique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\develops\sensitivewaldstandorteCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F964D44-4746-4924-91BC-8C9B61A4D769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C5199E-8C25-49B2-89E0-B29ED08A2CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
     <t>66</t>
   </si>
   <si>
-    <t>index</t>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,27 +805,24 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -833,69 +830,69 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>531</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>1077</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -903,41 +900,44 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>413</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -945,52 +945,55 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -998,91 +1001,97 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>21</v>
+        <v>237</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>26</v>
+        <v>365</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
         <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1090,24 +1099,27 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>37</v>
+        <v>199</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>40</v>
+        <v>1170</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
@@ -1115,38 +1127,41 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>47</v>
+        <v>1610</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1154,91 +1169,97 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>50</v>
+        <v>1241</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
         <v>52</v>
       </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" t="s">
-        <v>48</v>
-      </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>56</v>
+        <v>188</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
@@ -1246,13 +1267,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>58</v>
+        <v>358</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -1260,211 +1281,202 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>62</v>
+        <v>337</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>77</v>
+        <v>1996</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>83</v>
+        <v>4489</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>90</v>
+        <v>2431</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>97</v>
+        <v>152</v>
+      </c>
+      <c r="B42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>105</v>
+        <v>196</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>110</v>
+        <v>3331</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
-      </c>
-      <c r="D46" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>116</v>
+        <v>359</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="D47" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D49" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B50" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>129</v>
+        <v>2750</v>
       </c>
       <c r="B51" t="s">
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>70</v>
+        <v>123</v>
       </c>
       <c r="D51" t="s">
         <v>5</v>
@@ -1472,63 +1484,69 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>133</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>152</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>19</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>196</v>
+        <v>2434</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>76</v>
+        <v>120</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>199</v>
+        <v>253</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -1536,13 +1554,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>222</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="D57" t="s">
         <v>5</v>
@@ -1550,41 +1568,41 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D58" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>237</v>
+        <v>2512</v>
       </c>
       <c r="B59" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>252</v>
+        <v>498</v>
       </c>
       <c r="B60" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="D60" t="s">
         <v>5</v>
@@ -1592,13 +1610,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>253</v>
+        <v>1150</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="D61" t="s">
         <v>5</v>
@@ -1606,13 +1624,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>272</v>
+        <v>8734</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="D62" t="s">
         <v>5</v>
@@ -1620,267 +1638,270 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>297</v>
+        <v>10109</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>86</v>
+        <v>127</v>
+      </c>
+      <c r="D63" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>318</v>
+        <v>559</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C64" t="s">
-        <v>88</v>
-      </c>
-      <c r="D64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>337</v>
+        <v>226</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D65" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
+        <v>101</v>
+      </c>
+      <c r="B66" t="s">
+        <v>62</v>
+      </c>
+      <c r="C66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>901</v>
+      </c>
+      <c r="B67" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>37</v>
+      </c>
+      <c r="B68" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>56</v>
+      </c>
+      <c r="B69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69" t="s">
+        <v>50</v>
+      </c>
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>22231</v>
+      </c>
+      <c r="B70" t="s">
+        <v>130</v>
+      </c>
+      <c r="C70" t="s">
+        <v>130</v>
+      </c>
+      <c r="D70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>133</v>
+      </c>
+      <c r="B71" t="s">
+        <v>71</v>
+      </c>
+      <c r="C71" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
         <v>344</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B72" t="s">
         <v>71</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C72" t="s">
         <v>71</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D72" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>350</v>
-      </c>
-      <c r="B67" t="s">
-        <v>90</v>
-      </c>
-      <c r="C67" t="s">
-        <v>91</v>
-      </c>
-      <c r="D67" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>355</v>
-      </c>
-      <c r="B68" t="s">
-        <v>92</v>
-      </c>
-      <c r="C68" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>358</v>
-      </c>
-      <c r="B69" t="s">
-        <v>93</v>
-      </c>
-      <c r="C69" t="s">
-        <v>93</v>
-      </c>
-      <c r="D69" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>359</v>
-      </c>
-      <c r="B70" t="s">
-        <v>94</v>
-      </c>
-      <c r="C70" t="s">
-        <v>94</v>
-      </c>
-      <c r="D70" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>12172</v>
+      </c>
+      <c r="B73" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73" t="s">
+        <v>129</v>
+      </c>
+      <c r="D73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>116</v>
+      </c>
+      <c r="B74" t="s">
+        <v>65</v>
+      </c>
+      <c r="C74" t="s">
+        <v>66</v>
+      </c>
+      <c r="D74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>571</v>
+      </c>
+      <c r="B75" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>1</v>
+      </c>
+      <c r="B76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>83</v>
+      </c>
+      <c r="B77" t="s">
+        <v>58</v>
+      </c>
+      <c r="C77" t="s">
+        <v>59</v>
+      </c>
+      <c r="D77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>1813</v>
+      </c>
+      <c r="B78" t="s">
+        <v>58</v>
+      </c>
+      <c r="C78" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>365</v>
-      </c>
-      <c r="B71" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" t="s">
-        <v>95</v>
-      </c>
-      <c r="D71" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>369</v>
-      </c>
-      <c r="B72" t="s">
-        <v>40</v>
-      </c>
-      <c r="C72" t="s">
-        <v>96</v>
-      </c>
-      <c r="D72" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>413</v>
-      </c>
-      <c r="B73" t="s">
-        <v>97</v>
-      </c>
-      <c r="C73" t="s">
-        <v>98</v>
-      </c>
-      <c r="D73" t="s">
-        <v>5</v>
-      </c>
-      <c r="E73" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>489</v>
-      </c>
-      <c r="B74" t="s">
-        <v>99</v>
-      </c>
-      <c r="C74" t="s">
-        <v>100</v>
-      </c>
-      <c r="D74" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>498</v>
-      </c>
-      <c r="B75" t="s">
-        <v>101</v>
-      </c>
-      <c r="C75" t="s">
-        <v>101</v>
-      </c>
-      <c r="D75" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>517</v>
-      </c>
-      <c r="B76" t="s">
-        <v>102</v>
-      </c>
-      <c r="C76" t="s">
-        <v>102</v>
-      </c>
-      <c r="D76" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>531</v>
-      </c>
-      <c r="B77" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D77" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>559</v>
-      </c>
-      <c r="B78" t="s">
-        <v>104</v>
-      </c>
-      <c r="C78" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>571</v>
-      </c>
       <c r="B79" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C79" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D79" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>901</v>
+        <v>318</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C80" t="s">
-        <v>105</v>
+        <v>88</v>
+      </c>
+      <c r="D80" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>1077</v>
+        <v>272</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="D81" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>1150</v>
+        <v>26</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="C82" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="D82" t="s">
         <v>5</v>
@@ -1888,13 +1909,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>1170</v>
+        <v>110</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="C83" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="D83" t="s">
         <v>5</v>
@@ -1902,13 +1923,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>1191</v>
+        <v>2681</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="C84" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D84" t="s">
         <v>9</v>
@@ -1916,27 +1937,27 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>1241</v>
+        <v>73</v>
       </c>
       <c r="B85" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C85" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="D85" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>1610</v>
+        <v>350</v>
       </c>
       <c r="B86" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="C86" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="D86" t="s">
         <v>9</v>
@@ -1944,27 +1965,30 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>1813</v>
+        <v>489</v>
       </c>
       <c r="B87" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="C87" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D87" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>1996</v>
+        <v>1191</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C88" t="s">
-        <v>115</v>
+        <v>109</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1983,69 +2007,69 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>2431</v>
+        <v>517</v>
       </c>
       <c r="B90" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C90" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D90" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>2434</v>
+        <v>47</v>
       </c>
       <c r="B91" t="s">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="C91" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="D91" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>2512</v>
+        <v>369</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="C92" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="D92" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>2681</v>
+        <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>122</v>
+        <v>16</v>
       </c>
       <c r="C93" t="s">
-        <v>122</v>
+        <v>16</v>
       </c>
       <c r="D93" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>2750</v>
+        <v>52</v>
       </c>
       <c r="B94" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C94" t="s">
-        <v>123</v>
+        <v>48</v>
       </c>
       <c r="D94" t="s">
         <v>5</v>
@@ -2053,86 +2077,65 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>3331</v>
+        <v>252</v>
       </c>
       <c r="B95" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C95" t="s">
-        <v>124</v>
+        <v>82</v>
+      </c>
+      <c r="D95" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>4489</v>
+        <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>125</v>
+        <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>125</v>
+        <v>12</v>
       </c>
       <c r="D96" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>8734</v>
-      </c>
-      <c r="B97" t="s">
-        <v>126</v>
+        <v>29</v>
       </c>
       <c r="C97" t="s">
-        <v>126</v>
-      </c>
-      <c r="D97" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>10109</v>
-      </c>
-      <c r="B98" t="s">
-        <v>127</v>
+        <v>55</v>
       </c>
       <c r="C98" t="s">
-        <v>127</v>
-      </c>
-      <c r="D98" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>12172</v>
-      </c>
-      <c r="B99" t="s">
-        <v>128</v>
-      </c>
-      <c r="C99" t="s">
-        <v>129</v>
-      </c>
-      <c r="D99" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>22231</v>
-      </c>
-      <c r="B100" t="s">
-        <v>130</v>
+        <v>297</v>
       </c>
       <c r="C100" t="s">
-        <v>130</v>
-      </c>
-      <c r="D100" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E100">
+    <sortCondition ref="B1:B100"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>